<commit_message>
Code refracted, implemented ImethodIneterceptor and dataprovide
</commit_message>
<xml_diff>
--- a/src/test/resources/resources/excel/testdata.xlsx
+++ b/src/test/resources/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\alfaDOCK_GPN\src\test\resources\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9ADF74-E818-4B47-BE10-FCD80B2F6B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82F9697-A94D-4F7F-A4E5-9EE75BA14020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
   <si>
     <t>testname</t>
   </si>
@@ -42,9 +43,6 @@
     <t>count</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>test1</t>
   </si>
   <si>
@@ -58,14 +56,220 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>To check weather the use can succesfully login and Logout</t>
+  </si>
+  <si>
+    <t>Dummy test for pass test</t>
+  </si>
+  <si>
+    <t>Dummy test for pass test 2</t>
+  </si>
+  <si>
+    <t>Dummy test for pass fail</t>
+  </si>
+  <si>
+    <t>Dummy test for pass skip</t>
+  </si>
+  <si>
+    <t>alfaDOCKLoginTest</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>customerPassword</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>userPassword</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>sakae</t>
+  </si>
+  <si>
+    <t>service701</t>
+  </si>
+  <si>
+    <t>unozawa</t>
+  </si>
+  <si>
+    <t>nakanoya</t>
+  </si>
+  <si>
+    <t>kms01</t>
+  </si>
+  <si>
+    <t>j2019imr</t>
+  </si>
+  <si>
+    <t>AlfaTKG</t>
+  </si>
+  <si>
+    <t>AD15a18</t>
+  </si>
+  <si>
+    <t>umeda</t>
+  </si>
+  <si>
+    <t>umeda123</t>
+  </si>
+  <si>
+    <t>Sanken</t>
+  </si>
+  <si>
+    <t>sanken123</t>
+  </si>
+  <si>
+    <t>axis</t>
+  </si>
+  <si>
+    <t>axis10061952</t>
+  </si>
+  <si>
+    <t>tanakasangyo</t>
+  </si>
+  <si>
+    <t>Makabe-A</t>
+  </si>
+  <si>
+    <t>makabea123</t>
+  </si>
+  <si>
+    <t>Makabe-I</t>
+  </si>
+  <si>
+    <t>makabei123</t>
+  </si>
+  <si>
+    <t>sinsyo</t>
+  </si>
+  <si>
+    <t>sinsyo888</t>
+  </si>
+  <si>
+    <t>yoshimi</t>
+  </si>
+  <si>
+    <t>akaishik</t>
+  </si>
+  <si>
+    <t>Musasi-kogyo</t>
+  </si>
+  <si>
+    <t>musasi123</t>
+  </si>
+  <si>
+    <t>daitoh-t1966</t>
+  </si>
+  <si>
+    <t>dt9969316</t>
+  </si>
+  <si>
+    <t>makino</t>
+  </si>
+  <si>
+    <t>makino123</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>KANEYOSHI</t>
+  </si>
+  <si>
+    <t>KANE</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>asuna</t>
+  </si>
+  <si>
+    <t>ohashi</t>
+  </si>
+  <si>
+    <t>ohashi1916</t>
+  </si>
+  <si>
+    <t>sds</t>
+  </si>
+  <si>
+    <t>sakaiss</t>
+  </si>
+  <si>
+    <t>sss1970</t>
+  </si>
+  <si>
+    <t>eiwakiko</t>
+  </si>
+  <si>
+    <t>Reborn-eiwa</t>
+  </si>
+  <si>
+    <t>SAMETA</t>
+  </si>
+  <si>
+    <t>SAMETA123</t>
+  </si>
+  <si>
+    <t>ntc3119</t>
+  </si>
+  <si>
+    <t>shinkousha</t>
+  </si>
+  <si>
+    <t>iwa</t>
+  </si>
+  <si>
+    <t>iwa123</t>
+  </si>
+  <si>
+    <t>0037</t>
+  </si>
+  <si>
+    <t>9771836</t>
+  </si>
+  <si>
+    <t>7586</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>7241</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>77727</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,10 +297,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -380,18 +596,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="63" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -413,45 +627,694 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C533EB-FD6A-4668-B073-71D0EC963980}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>